<commit_message>
Updated Code to Produce Graphical Representation
</commit_message>
<xml_diff>
--- a/Config/Config.xlsx
+++ b/Config/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pritish Sanyal\Documents\UiPath\QueueReportGeneration\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D916A41-15E0-4BA1-B1F6-ED4746ED1DB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D93A168-F9CF-479F-B2F5-F36B0B5B5861}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -76,28 +76,28 @@
     <t>ReportFields</t>
   </si>
   <si>
+    <t>EmailCredentials</t>
+  </si>
+  <si>
+    <t>The Fields which are required in the Queue Report</t>
+  </si>
+  <si>
+    <t>ReportBackDay</t>
+  </si>
+  <si>
+    <t>The Number of days past from today for which the report is to be generated</t>
+  </si>
+  <si>
+    <t>C:\Project\QueueReports</t>
+  </si>
+  <si>
+    <t>pritish.sanyal23@gmail.com; mailme.pritish@gmail.com;</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
     <t>ItemKey,Reference,Status,StartedTime,ExceptionTime,LastUpdated,ExceptionType,ExceptionReason,ExceptionDetails</t>
-  </si>
-  <si>
-    <t>EmailCredentials</t>
-  </si>
-  <si>
-    <t>The Fields which are required in the Queue Report</t>
-  </si>
-  <si>
-    <t>ReportBackDay</t>
-  </si>
-  <si>
-    <t>The Number of days past from today for which the report is to be generated</t>
-  </si>
-  <si>
-    <t>C:\Project\QueueReports</t>
-  </si>
-  <si>
-    <t>API;CustomerSecurityHash</t>
-  </si>
-  <si>
-    <t>pritish.sanyal23@gmail.com; mailme.pritish@gmail.com;</t>
   </si>
 </sst>
 </file>
@@ -189,8 +189,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -519,8 +521,8 @@
       <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>23</v>
+      <c r="B4" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>11</v>
@@ -531,7 +533,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>13</v>
@@ -539,7 +541,7 @@
     </row>
     <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>6</v>
@@ -553,21 +555,21 @@
         <v>15</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="11">
+        <v>100</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>19</v>
-      </c>
-      <c r="B8" s="10">
-        <v>1</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>